<commit_message>
- change Tiktok CashSalesImport code to 325-000 - update test data
</commit_message>
<xml_diff>
--- a/tests/tiktok/data.input/tiktok.monthly.cashsales.record.sample.xlsx
+++ b/tests/tiktok/data.input/tiktok.monthly.cashsales.record.sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\mlcmi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\cardeco\tests\tiktok\data.input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{313A7F3E-B800-4FD3-AD07-61246FAD07F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C20BE60-AD73-4FA9-9FC4-7DC19D3650FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFDD22F8-02DF-4E0F-9598-AFB6056EA166}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>TRACKING NUMBER</t>
   </si>
@@ -123,6 +123,114 @@
   </si>
   <si>
     <t xml:space="preserve">577052873750055046	</t>
+  </si>
+  <si>
+    <t>CS-78798</t>
+  </si>
+  <si>
+    <t>HT-CLASSIC PVC MAT BAKUL MOTOR (36MM X30MM) (13MM) - BLACK</t>
+  </si>
+  <si>
+    <t>CM-36X30-BLK</t>
+  </si>
+  <si>
+    <t>HT-CLASSIC PVC MAT BAKUL MOTOR (36MM X30MM) (13MM) - BLACK BLUE</t>
+  </si>
+  <si>
+    <t>CM-36X30-BL</t>
+  </si>
+  <si>
+    <t>CS-78799</t>
+  </si>
+  <si>
+    <t>BOSCH WIPER 21" (SINGLE PACK)</t>
+  </si>
+  <si>
+    <t>BW-0012</t>
+  </si>
+  <si>
+    <t>BOSCH WIPER 14" (SINGLE PACK)</t>
+  </si>
+  <si>
+    <t>BW-0009</t>
+  </si>
+  <si>
+    <t>TRUST WINDSCREEN CLEANER (120ml) - T4W</t>
+  </si>
+  <si>
+    <t>CCP-0116</t>
+  </si>
+  <si>
+    <t>BOSCH WIPER 24" (SINGLE PACK)</t>
+  </si>
+  <si>
+    <t>BW-0014</t>
+  </si>
+  <si>
+    <t>CARGO TRAY (PERODUA) AXIA 2023 NEW (LOCAL) BTK021</t>
+  </si>
+  <si>
+    <t>IN-0798-23</t>
+  </si>
+  <si>
+    <t>CS-78825</t>
+  </si>
+  <si>
+    <t>CS-78826</t>
+  </si>
+  <si>
+    <t>CARGO TRAY (NISSAN) ALMERA 12-19 (LOCAL/ABS)</t>
+  </si>
+  <si>
+    <t>IN-0733-L</t>
+  </si>
+  <si>
+    <t>CS-78827</t>
+  </si>
+  <si>
+    <t>CS-78828</t>
+  </si>
+  <si>
+    <t>685309128934</t>
+  </si>
+  <si>
+    <t>685376584942</t>
+  </si>
+  <si>
+    <t>685406029116</t>
+  </si>
+  <si>
+    <t>685411522183</t>
+  </si>
+  <si>
+    <t>685465191895</t>
+  </si>
+  <si>
+    <t>685478217963</t>
+  </si>
+  <si>
+    <t>685421346920</t>
+  </si>
+  <si>
+    <t>685454362900</t>
+  </si>
+  <si>
+    <t>577067123432982942</t>
+  </si>
+  <si>
+    <t>577067466836248720</t>
+  </si>
+  <si>
+    <t>577149320715733503</t>
+  </si>
+  <si>
+    <t>577151311291320742</t>
+  </si>
+  <si>
+    <t>577153451999660335</t>
+  </si>
+  <si>
+    <t>577155096869964604</t>
   </si>
 </sst>
 </file>
@@ -198,11 +306,7 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -223,9 +327,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -234,6 +335,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -549,19 +657,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4066C0F-500E-4012-907C-8B2F015741E8}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
@@ -569,186 +677,498 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="10">
-        <v>685309128934</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="B2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="8">
         <v>44984</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="9">
         <v>44980</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="11">
         <v>41.2</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="14">
+      <c r="K2" s="11">
         <v>5.6</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="10">
-        <v>685376584942</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="B3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="8">
         <v>44984</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>44983</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="11">
         <v>51.2</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="14">
+      <c r="K3" s="11">
         <v>5.6</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>44983</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="11">
         <v>65</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="14">
+      <c r="K4" s="11">
         <v>6.3</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="14">
+        <v>44995</v>
+      </c>
+      <c r="D5" s="9">
+        <v>44988</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5">
+        <v>7.5</v>
+      </c>
+      <c r="M5">
+        <v>0.74</v>
+      </c>
+      <c r="N5">
+        <v>14.26</v>
+      </c>
+      <c r="O5">
+        <v>14.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="14">
+        <v>44995</v>
+      </c>
+      <c r="D6" s="9">
+        <v>44988</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="14">
+        <v>44992</v>
+      </c>
+      <c r="D7" s="9">
+        <v>44988</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7">
+        <v>13</v>
+      </c>
+      <c r="M7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N7">
+        <v>23.9</v>
+      </c>
+      <c r="O7">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="14">
+        <v>44992</v>
+      </c>
+      <c r="D8" s="9">
+        <v>44988</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="14">
+        <v>44992</v>
+      </c>
+      <c r="D9" s="9">
+        <v>44988</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="14">
+        <v>45015</v>
+      </c>
+      <c r="D10" s="9">
+        <v>45015</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10">
+        <v>14</v>
+      </c>
+      <c r="M10">
+        <v>2.23</v>
+      </c>
+      <c r="N10">
+        <v>53.77</v>
+      </c>
+      <c r="O10">
+        <v>53.77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="14">
+        <v>45015</v>
+      </c>
+      <c r="D11" s="9">
+        <v>45015</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="14">
+        <v>45015</v>
+      </c>
+      <c r="D12" s="9">
+        <v>45015</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="14">
+        <v>45015</v>
+      </c>
+      <c r="D13" s="9">
+        <v>45015</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="14">
+        <v>45016</v>
+      </c>
+      <c r="D14" s="9">
+        <v>45015</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14">
+        <v>48</v>
+      </c>
+      <c r="M14">
+        <v>1.47</v>
+      </c>
+      <c r="N14">
+        <v>46.53</v>
+      </c>
+      <c r="O14">
+        <v>46.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="14">
+        <v>45016</v>
+      </c>
+      <c r="D15" s="9">
+        <v>45016</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15">
+        <v>58</v>
+      </c>
+      <c r="M15">
+        <v>2.33</v>
+      </c>
+      <c r="N15">
+        <v>55.67</v>
+      </c>
+      <c r="O15">
+        <v>55.67</v>
+      </c>
+      <c r="P15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="14">
+        <v>45020</v>
+      </c>
+      <c r="D16" s="9">
+        <v>45016</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="M16">
+        <v>2.12</v>
+      </c>
+      <c r="N16">
+        <v>47.88</v>
+      </c>
+      <c r="O16">
+        <v>47.88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>